<commit_message>
Added first real conv_1d configuration
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>111.8305852413177</v>
+        <v>110.9189436435699</v>
       </c>
     </row>
     <row r="2">
@@ -450,34 +450,34 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18779.686</v>
+        <v>18816.2325</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18875</v>
+        <v>18832</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>18587</v>
+        <v>18622</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>18862</v>
+        <v>18830</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>18516</v>
+        <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6348.619</v>
+        <v>6412.6795</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6328</v>
+        <v>6491</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>6235</v>
+        <v>6334</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>6330</v>
+        <v>6464</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>6271</v>
+        <v>6301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added combined convolutional neural network
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>110.9189436435699</v>
+        <v>162.5768232345581</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18816.2325</v>
+        <v>18814.8955</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18832</v>
+        <v>17451</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,10 +465,10 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6412.6795</v>
+        <v>6411.1545</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6491</v>
+        <v>6410</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>6334</v>

</xml_diff>

<commit_message>
Implemented combined convnet 2d
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>162.5768232345581</v>
+        <v>157.5051493644714</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18814.8955</v>
+        <v>18813.4895</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>17451</v>
+        <v>17525</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,10 +465,10 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6411.1545</v>
+        <v>6412.021</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6410</v>
+        <v>6455</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>6334</v>

</xml_diff>

<commit_message>
Implemented combined 1d neural net
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>157.5051493644714</v>
+        <v>158.370640039444</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18813.4895</v>
+        <v>18814.618</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>17525</v>
+        <v>18311</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,10 +465,10 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6412.021</v>
+        <v>6411.518</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6455</v>
+        <v>6359</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>6334</v>

</xml_diff>

<commit_message>
Reorganised log folder for tensorboard
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>158.370640039444</v>
+        <v>157.631557226181</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18814.618</v>
+        <v>18813.769</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18311</v>
+        <v>18280</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,10 +465,10 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6411.518</v>
+        <v>6412.029</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6359</v>
+        <v>6327</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>6334</v>

</xml_diff>

<commit_message>
Added validation loss/accuracy monitoring support
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>158.0527746677399</v>
+        <v>154.4054388999939</v>
       </c>
     </row>
     <row r="2">
@@ -392,7 +392,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>durations on test set</t>
+          <t>durations on validate set</t>
         </is>
       </c>
     </row>
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18814.4835</v>
+        <v>18814.897</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18508</v>
+        <v>18339</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,19 +465,19 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>6410.254</v>
+        <v>5945.339</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6378</v>
+        <v>5873</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>6334</v>
+        <v>5856</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>6464</v>
+        <v>5986</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>6301</v>
+        <v>5895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added variable to check whether futureResourceUtilisation matrix needs to be calculated for the convnet in use
</commit_message>
<xml_diff>
--- a/durations_psplib.xlsx
+++ b/durations_psplib.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>154.4054388999939</v>
+        <v>693.0009875297546</v>
       </c>
     </row>
     <row r="2">
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18814.897</v>
+        <v>18813.014</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18339</v>
+        <v>18746</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>18622</v>
@@ -465,10 +465,10 @@
         <v>18589</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>5945.339</v>
+        <v>5946.6485</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>5873</v>
+        <v>5885</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>5856</v>

</xml_diff>